<commit_message>
Correcion casos de prueba
</commit_message>
<xml_diff>
--- a/TPO - TC-PE-54.xlsx
+++ b/TPO - TC-PE-54.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gazza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Facultad\Testing de Apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7D61F14-B01C-4AEC-A08E-CB3625D3BBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0904DFCB-EA37-4E3D-BD66-C16E5CAB001C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
   </bookViews>
   <sheets>
     <sheet name="TC - Template 1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="72">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -158,18 +158,12 @@
     <t>PE-54</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify </t>
-  </si>
-  <si>
     <t>Mail = asd@gmail.com</t>
   </si>
   <si>
     <t>Pass = 123456</t>
   </si>
   <si>
-    <t>Usuario quiere iniciar sesion</t>
-  </si>
-  <si>
     <t>Acceso a internet</t>
   </si>
   <si>
@@ -213,6 +207,54 @@
   </si>
   <si>
     <t xml:space="preserve">Se bloquea al usuario </t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>Pass = asd123</t>
+  </si>
+  <si>
+    <t>Mail = asd123@gmail.com</t>
+  </si>
+  <si>
+    <t>Mail = asd19asd@gmail.com</t>
+  </si>
+  <si>
+    <t>TC-02</t>
+  </si>
+  <si>
+    <t>TC-03</t>
+  </si>
+  <si>
+    <t>TC-04</t>
+  </si>
+  <si>
+    <t>Usuario intenta iniciar sesion mas de 3 veces con una contraseña incorrecta.</t>
+  </si>
+  <si>
+    <t>Usuario quiere iniciar sesion con contraseña incorrecta.</t>
+  </si>
+  <si>
+    <t>Usuario quiere iniciar sesion con un mail incorrecto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario quiere iniciar sesion con mail y contraseña correctos. </t>
+  </si>
+  <si>
+    <t>Se prueba el inicio de sesion</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -346,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -517,17 +559,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -627,7 +658,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -659,13 +690,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -684,9 +711,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -705,80 +729,77 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1100,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9261CE-AC9B-4CCB-B585-79CAB2707733}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,18 +1142,18 @@
     <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E1" s="47"/>
     </row>
@@ -1140,29 +1161,32 @@
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="1:23" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11">
-        <v>2.1</v>
+      <c r="D3" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>56</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1182,11 +1206,11 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>37</v>
+      <c r="B5" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1208,7 +1232,7 @@
     </row>
     <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1222,35 +1246,35 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="3"/>
@@ -1260,244 +1284,244 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
       <c r="B11" s="3"/>
       <c r="F11" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="B13" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="G14" s="43" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="G14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:23" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41" t="s">
+      <c r="H15" s="35"/>
+      <c r="I15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41" t="s">
+      <c r="J15" s="35"/>
+      <c r="K15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41" t="s">
+      <c r="L15" s="35"/>
+      <c r="M15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="41"/>
+      <c r="N15" s="35"/>
     </row>
     <row r="16" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="44" t="s">
+      <c r="H16" s="37"/>
+      <c r="I16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="44" t="s">
+      <c r="J16" s="37"/>
+      <c r="K16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="45"/>
-      <c r="M16" s="44" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="48" t="s">
+      <c r="C17" s="39"/>
+      <c r="D17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="G17" s="14" t="s">
+      <c r="E17" s="41"/>
+      <c r="G17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>1</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="G18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>2</v>
+      </c>
+      <c r="B19" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="39" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="G18" s="16" t="s">
+      <c r="E19" s="43"/>
+      <c r="G19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="L19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="17" t="s">
+      <c r="M19" s="14"/>
+      <c r="N19" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>2</v>
-      </c>
-      <c r="B19" s="39" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>3</v>
+      </c>
+      <c r="B20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="G19" s="16" t="s">
+      <c r="E20" s="43"/>
+      <c r="G20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17" t="s">
+      <c r="M20" s="14"/>
+      <c r="N20" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>3</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="40"/>
-      <c r="G20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>4</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="40"/>
+      <c r="B21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="43"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
       <c r="I21" s="5"/>
@@ -1508,11 +1532,11 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
       <c r="I22" s="5"/>
@@ -1523,11 +1547,11 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
       <c r="G23" s="5"/>
       <c r="H23" s="3"/>
       <c r="I23" s="5"/>
@@ -1538,77 +1562,77 @@
       <c r="N23" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42" t="s">
+      <c r="H25" s="44"/>
+      <c r="I25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42" t="s">
+      <c r="L25" s="44"/>
+      <c r="M25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="42"/>
+      <c r="N25" s="44"/>
     </row>
     <row r="26" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38" t="s">
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
     </row>
     <row r="27" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
     </row>
     <row r="28" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
     </row>
     <row r="29" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
     </row>
     <row r="30" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
@@ -1659,6 +1683,8 @@
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="M15:N15"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1669,8 +1695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3CCAC7-6C0E-44CD-ADA1-CF7A0722318C}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,48 +1716,51 @@
     <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E1" s="47"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="1:23" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11">
-        <v>2.1</v>
+      <c r="D3" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>57</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1751,10 +1780,10 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="2"/>
@@ -1777,7 +1806,7 @@
     </row>
     <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1791,35 +1820,35 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="3"/>
@@ -1829,244 +1858,244 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
       <c r="B11" s="3"/>
       <c r="F11" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="B13" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="G14" s="43" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="G14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:23" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41" t="s">
+      <c r="H15" s="35"/>
+      <c r="I15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41" t="s">
+      <c r="J15" s="35"/>
+      <c r="K15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41" t="s">
+      <c r="L15" s="35"/>
+      <c r="M15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="41"/>
+      <c r="N15" s="35"/>
     </row>
     <row r="16" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="44" t="s">
+      <c r="H16" s="37"/>
+      <c r="I16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="44" t="s">
+      <c r="J16" s="37"/>
+      <c r="K16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="45"/>
-      <c r="M16" s="44" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="48" t="s">
+      <c r="C17" s="39"/>
+      <c r="D17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="G17" s="14" t="s">
+      <c r="E17" s="41"/>
+      <c r="G17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>1</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="G18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>2</v>
+      </c>
+      <c r="B19" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="39" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="G18" s="16" t="s">
+      <c r="E19" s="43"/>
+      <c r="G19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="L19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="17" t="s">
+      <c r="M19" s="14"/>
+      <c r="N19" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>2</v>
-      </c>
-      <c r="B19" s="39" t="s">
+    <row r="20" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>3</v>
+      </c>
+      <c r="B20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="40"/>
-      <c r="G19" s="16" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="43"/>
+      <c r="G20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17" t="s">
+      <c r="M20" s="14"/>
+      <c r="N20" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>3</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="40"/>
-      <c r="G20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>4</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="40"/>
+      <c r="B21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="43"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
       <c r="I21" s="5"/>
@@ -2077,11 +2106,11 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
       <c r="I22" s="5"/>
@@ -2092,11 +2121,11 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
       <c r="G23" s="5"/>
       <c r="H23" s="3"/>
       <c r="I23" s="5"/>
@@ -2107,80 +2136,80 @@
       <c r="N23" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42" t="s">
+      <c r="H25" s="44"/>
+      <c r="I25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42" t="s">
+      <c r="L25" s="44"/>
+      <c r="M25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="42"/>
+      <c r="N25" s="44"/>
     </row>
     <row r="26" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38" t="s">
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
     </row>
     <row r="27" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
     </row>
     <row r="28" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
     </row>
     <row r="29" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
     </row>
     <row r="30" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B17:C17"/>
@@ -2194,16 +2223,18 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M29:N29"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I25:J25"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M29:N29"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K25:L25"/>
@@ -2241,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AB1882-61D6-4204-B228-A3C3F2CFE2ED}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:E21"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2281,7 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="2.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
@@ -2262,18 +2293,18 @@
     <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E1" s="47"/>
     </row>
@@ -2281,30 +2312,31 @@
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11">
-        <v>2.1</v>
-      </c>
+      <c r="D3" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="47"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="I3" s="1"/>
@@ -2323,10 +2355,10 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="2"/>
@@ -2349,7 +2381,7 @@
     </row>
     <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -2363,35 +2395,35 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="3"/>
@@ -2401,244 +2433,244 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
       <c r="B11" s="3"/>
       <c r="F11" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="B13" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="G14" s="43" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="G14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:23" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41" t="s">
+      <c r="H15" s="35"/>
+      <c r="I15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41" t="s">
+      <c r="J15" s="35"/>
+      <c r="K15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41" t="s">
+      <c r="L15" s="35"/>
+      <c r="M15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="41"/>
+      <c r="N15" s="35"/>
     </row>
     <row r="16" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="44" t="s">
+      <c r="H16" s="37"/>
+      <c r="I16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="44" t="s">
+      <c r="J16" s="37"/>
+      <c r="K16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="45"/>
-      <c r="M16" s="44" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="48" t="s">
+      <c r="C17" s="39"/>
+      <c r="D17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="G17" s="14" t="s">
+      <c r="E17" s="41"/>
+      <c r="G17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>1</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="G18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>2</v>
+      </c>
+      <c r="B19" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="39" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="G18" s="16" t="s">
+      <c r="E19" s="43"/>
+      <c r="G19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="L19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="17" t="s">
+      <c r="M19" s="14"/>
+      <c r="N19" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>2</v>
-      </c>
-      <c r="B19" s="39" t="s">
+    <row r="20" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>3</v>
+      </c>
+      <c r="B20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="40"/>
-      <c r="G19" s="16" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="43"/>
+      <c r="G20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17" t="s">
+      <c r="M20" s="14"/>
+      <c r="N20" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>3</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="40"/>
-      <c r="G20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="21" spans="1:14" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>4</v>
       </c>
-      <c r="B21" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="40"/>
+      <c r="B21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="43"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
       <c r="I21" s="5"/>
@@ -2649,11 +2681,11 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
       <c r="I22" s="5"/>
@@ -2664,11 +2696,11 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
       <c r="G23" s="5"/>
       <c r="H23" s="3"/>
       <c r="I23" s="5"/>
@@ -2679,80 +2711,80 @@
       <c r="N23" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42" t="s">
+      <c r="H25" s="44"/>
+      <c r="I25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42" t="s">
+      <c r="L25" s="44"/>
+      <c r="M25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="42"/>
+      <c r="N25" s="44"/>
     </row>
     <row r="26" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38" t="s">
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
     </row>
     <row r="27" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
     </row>
     <row r="28" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
     </row>
     <row r="29" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
     </row>
     <row r="30" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
@@ -2803,6 +2835,8 @@
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="M15:N15"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2813,17 +2847,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7A5110-67BD-425F-B2CE-4E92CBBC401D}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -2834,48 +2869,51 @@
     <col min="14" max="14" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E1" s="47"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="46" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="1:23" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11">
-        <v>2.1</v>
+      <c r="D3" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>59</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2895,10 +2933,10 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="2"/>
@@ -2921,7 +2959,7 @@
     </row>
     <row r="6" spans="1:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -2935,35 +2973,35 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="3"/>
@@ -2973,244 +3011,244 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
       <c r="B11" s="3"/>
       <c r="F11" s="1"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="34"/>
+      <c r="B13" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:23" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="G14" s="43" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="G14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:23" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21"/>
+      <c r="D15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41" t="s">
+      <c r="H15" s="35"/>
+      <c r="I15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41" t="s">
+      <c r="J15" s="35"/>
+      <c r="K15" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41" t="s">
+      <c r="L15" s="35"/>
+      <c r="M15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="41"/>
+      <c r="N15" s="35"/>
     </row>
     <row r="16" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="44" t="s">
+      <c r="G16" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="44" t="s">
+      <c r="H16" s="37"/>
+      <c r="I16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="44" t="s">
+      <c r="J16" s="37"/>
+      <c r="K16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="45"/>
-      <c r="M16" s="44" t="s">
+      <c r="L16" s="37"/>
+      <c r="M16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="45"/>
+      <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14" ht="26.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="48" t="s">
+      <c r="C17" s="39"/>
+      <c r="D17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="49"/>
-      <c r="G17" s="14" t="s">
+      <c r="E17" s="41"/>
+      <c r="G17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L17" s="14" t="s">
+      <c r="L17" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>1</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="43"/>
+      <c r="G18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>2</v>
+      </c>
+      <c r="B19" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="39" t="s">
+      <c r="C19" s="43"/>
+      <c r="D19" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="G18" s="16" t="s">
+      <c r="E19" s="43"/>
+      <c r="G19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="I19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="L19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="16"/>
-      <c r="N18" s="17" t="s">
+      <c r="M19" s="14"/>
+      <c r="N19" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>2</v>
-      </c>
-      <c r="B19" s="39" t="s">
+    <row r="20" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>3</v>
+      </c>
+      <c r="B20" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="40"/>
-      <c r="G19" s="16" t="s">
+      <c r="C20" s="43"/>
+      <c r="D20" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="43"/>
+      <c r="G20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="N19" s="17" t="s">
+      <c r="M20" s="14"/>
+      <c r="N20" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
-        <v>3</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="40"/>
-      <c r="G20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M20" s="16"/>
-      <c r="N20" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="21" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>4</v>
       </c>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="43"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
       <c r="I21" s="5"/>
@@ -3221,11 +3259,11 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="40"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
       <c r="G22" s="5"/>
       <c r="H22" s="3"/>
       <c r="I22" s="5"/>
@@ -3236,11 +3274,11 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
       <c r="G23" s="5"/>
       <c r="H23" s="3"/>
       <c r="I23" s="5"/>
@@ -3251,80 +3289,80 @@
       <c r="N23" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42" t="s">
+      <c r="H25" s="44"/>
+      <c r="I25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42" t="s">
+      <c r="L25" s="44"/>
+      <c r="M25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="N25" s="42"/>
+      <c r="N25" s="44"/>
     </row>
     <row r="26" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38" t="s">
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="38"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="45"/>
     </row>
     <row r="27" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="45"/>
     </row>
     <row r="28" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>53</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="45"/>
     </row>
     <row r="29" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
     </row>
     <row r="30" spans="1:14" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="52">
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="K29:L29"/>
@@ -3375,6 +3413,8 @@
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="M15:N15"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>